<commit_message>
extract data from new data file
</commit_message>
<xml_diff>
--- a/beta/matlab/data/NewImageCoords1234.xlsx
+++ b/beta/matlab/data/NewImageCoords1234.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KArin\git\U-TRACKR\beta\matlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48086B9D-D742-45F4-B008-61801CFE37EB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F19846-3DBD-4221-818F-67D6CB110956}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="8228" xr2:uid="{139A0A07-9EB3-4718-9D9D-96366C1B3595}"/>
   </bookViews>
@@ -25,7 +25,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>img1x</t>
+  </si>
+  <si>
+    <t>img1y</t>
+  </si>
+  <si>
+    <t>img2x</t>
+  </si>
+  <si>
+    <t>img2y</t>
+  </si>
+  <si>
+    <t>img3x</t>
+  </si>
+  <si>
+    <t>img3y</t>
+  </si>
+  <si>
+    <t>img4x</t>
+  </si>
+  <si>
+    <t>img4y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,14 +400,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C06788-1C44-4673-87EE-CA25278268C9}">
-  <dimension ref="B2:I5"/>
+  <dimension ref="B1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B2">
         <v>2119</v>

</xml_diff>